<commit_message>
fixed the optuna hyperparameter functionality. ran and saved the result to reports
</commit_message>
<xml_diff>
--- a/reports/model_comparison_table_1.xlsx
+++ b/reports/model_comparison_table_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,26 @@
           <t>test_f1_std</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>train_auc_mean</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>train_auc_std</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>test_auc_mean</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>test_auc_std</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -462,16 +482,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6400478898533373</v>
+        <v>0.6657288237054775</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01898551092140342</v>
+        <v>0.02030859421041251</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6313397129186603</v>
+        <v>0.6294258373205742</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01861422360184392</v>
+        <v>0.01489030269817745</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.8633649170189001</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.02419685626886079</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8226899596653634</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.01229899196398712</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +513,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6028135288835678</v>
+        <v>0.6484286141873691</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02715335152359586</v>
+        <v>0.002486989293964791</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5980861244019138</v>
+        <v>0.6296650717703349</v>
       </c>
       <c r="E3" t="n">
-        <v>0.01980017387230485</v>
+        <v>0.01682483346652369</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.8377362221948003</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.00515588624869271</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.8250505286560126</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.01405039152506807</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +544,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0.7585154145465429</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.02194213185177669</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6433014354066986</v>
+        <v>0.6504784688995214</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0157495508044333</v>
+        <v>0.01007628693236968</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9429673530162714</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0103405237850859</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8567615011325733</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.006371552262075229</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +575,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6970966776414247</v>
+        <v>0.7221191260101765</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01219047246086584</v>
+        <v>0.01081604556517469</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6495215311004785</v>
+        <v>0.6447368421052632</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01325540208344027</v>
+        <v>0.0148441072320465</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9081177555601091</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.00872448205911735</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.8477274261429854</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.009114870178775806</v>
       </c>
     </row>
     <row r="6">
@@ -538,16 +606,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.7339120023944927</v>
+        <v>0.7060161628255013</v>
       </c>
       <c r="C6" t="n">
-        <v>0.06486075795855746</v>
+        <v>0.02514317068757808</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6428229665071771</v>
+        <v>0.6464114832535885</v>
       </c>
       <c r="E6" t="n">
-        <v>0.01218922411756649</v>
+        <v>0.008777003027676644</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9017459306803971</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.01583270590270821</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.8548609096269795</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.009381170360451847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>